<commit_message>
updated demo data, made stock_location.name consistent with pv_pn.PNUser9
</commit_message>
<xml_diff>
--- a/protected/data/excel/stock_location.xlsx
+++ b/protected/data/excel/stock_location.xlsx
@@ -14,19 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
-  <si>
-    <t>active parts</t>
-  </si>
-  <si>
-    <t>passive parts</t>
-  </si>
-  <si>
-    <t>stock room 1</t>
-  </si>
-  <si>
-    <t>stock room 2</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>use_sublocation</t>
   </si>
@@ -38,6 +26,39 @@
   </si>
   <si>
     <t>sublocation_max</t>
+  </si>
+  <si>
+    <t>FINGOODS</t>
+  </si>
+  <si>
+    <t>ELEC-PCB</t>
+  </si>
+  <si>
+    <t>ELEC-COMPS</t>
+  </si>
+  <si>
+    <t>ELEC-WIRE</t>
+  </si>
+  <si>
+    <t>DOCS</t>
+  </si>
+  <si>
+    <t>SHOPSUP</t>
+  </si>
+  <si>
+    <t>MECH</t>
+  </si>
+  <si>
+    <t>SHIPPING</t>
+  </si>
+  <si>
+    <t>ELEC-CONNS</t>
+  </si>
+  <si>
+    <t>MECH-HW</t>
+  </si>
+  <si>
+    <t>YARD</t>
   </si>
 </sst>
 </file>
@@ -869,7 +890,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -883,21 +904,21 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="B2" s="1">
         <v>1</v>
@@ -906,12 +927,12 @@
         <v>1</v>
       </c>
       <c r="D2" s="1">
-        <v>100</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B3" s="1">
         <v>1</v>
@@ -920,12 +941,12 @@
         <v>1</v>
       </c>
       <c r="D3" s="1">
-        <v>100</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="B4" s="1">
         <v>1</v>
@@ -939,19 +960,120 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B5" s="1">
+        <v>1</v>
+      </c>
+      <c r="C5" s="1">
+        <v>1</v>
+      </c>
+      <c r="D5" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="1">
+        <v>1</v>
+      </c>
+      <c r="C6" s="1">
+        <v>1</v>
+      </c>
+      <c r="D6" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="1">
+        <v>1</v>
+      </c>
+      <c r="C7" s="1">
+        <v>1</v>
+      </c>
+      <c r="D7" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="1">
+        <v>1</v>
+      </c>
+      <c r="C8" s="1">
+        <v>1</v>
+      </c>
+      <c r="D8" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="1">
+        <v>1</v>
+      </c>
+      <c r="C9" s="1">
+        <v>1</v>
+      </c>
+      <c r="D9" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="1">
+        <v>1</v>
+      </c>
+      <c r="C10" s="1">
+        <v>1</v>
+      </c>
+      <c r="D10" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="1">
+        <v>1</v>
+      </c>
+      <c r="C11" s="1">
+        <v>1</v>
+      </c>
+      <c r="D11" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" s="1">
         <v>0</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C12" s="1">
         <v>0</v>
       </c>
-      <c r="D5" s="1">
+      <c r="D12" s="1">
         <v>0</v>
       </c>
     </row>
   </sheetData>
+  <sortState ref="A2:A11">
+    <sortCondition ref="A2"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>